<commit_message>
change file name and bugs
</commit_message>
<xml_diff>
--- a/Trials.xlsx
+++ b/Trials.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/155826a8f07387bf/GE_Drive/PhD/PhD Projects/codes/unimanual-codes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_79090697BD6138C2AB8FC3732DC7EA528BDDE913" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EDC605A-C3BC-447E-9B51-5FD7F7D089F7}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Template"/>
-    <sheet r:id="rId2" sheetId="2" name="Testing"/>
-    <sheet r:id="rId3" sheetId="3" name="Practice"/>
-    <sheet r:id="rId4" sheetId="4" name="Baseline"/>
-    <sheet r:id="rId5" sheetId="5" name="Exposure"/>
-    <sheet r:id="rId6" sheetId="6" name="Post"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing" sheetId="2" r:id="rId2"/>
+    <sheet name="Practice" sheetId="3" r:id="rId3"/>
+    <sheet name="Baseline" sheetId="4" r:id="rId4"/>
+    <sheet name="Exposure" sheetId="5" r:id="rId5"/>
+    <sheet name="Post" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="29">
   <si>
     <t>trial_num</t>
   </si>
@@ -69,10 +75,6 @@
     <t>Trial number</t>
   </si>
   <si>
-    <t>Target angle
-in degrees</t>
-  </si>
-  <si>
     <t>Target amplitude
 in degrees</t>
   </si>
@@ -85,16 +87,8 @@
 No feedback = 0</t>
   </si>
   <si>
-    <t>CW = 1
-CCW = -1</t>
-  </si>
-  <si>
     <t>Rotation = 1
 No rotation = 0</t>
-  </si>
-  <si>
-    <t>Rotation angle 
-in degrees</t>
   </si>
   <si>
     <t>clamp = 1
@@ -105,19 +99,37 @@
 in degrees</t>
   </si>
   <si>
-    <t>Vibration = 1
-No Vibration = 0</t>
+    <t>offset_direction</t>
   </si>
   <si>
-    <t>0=slice
-1=stop</t>
+    <t>forward = 1
+backward = -1</t>
+  </si>
+  <si>
+    <t>offset</t>
+  </si>
+  <si>
+    <t>offset_size</t>
+  </si>
+  <si>
+    <t>offset size 
+in degrees</t>
+  </si>
+  <si>
+    <t>clamp_direction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+No Vibration = 0
+Biceps = 1
+Triceps = 2
+Both = 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,12 +154,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdeebf7"/>
+        <fgColor rgb="FFDEEBF7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFfff2cc"/>
+        <fgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -185,59 +197,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -248,10 +257,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -289,71 +298,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -381,7 +390,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -404,11 +413,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -417,13 +426,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -433,7 +442,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -442,7 +451,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -451,7 +460,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -459,10 +468,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -527,247 +536,221 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="14" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="14" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="11" customWidth="1"/>
+    <col min="10" max="12" width="16.109375" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="8" t="s">
+      <c r="F1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5">
-      <c r="A2" s="9" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="K2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+      <c r="L2" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -775,31 +758,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +822,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -875,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -913,7 +898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -951,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -995,7 +980,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1003,23 +988,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,11 +1038,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1095,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1133,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1171,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1209,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1245,7 +1230,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1281,7 +1266,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1317,7 +1302,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1353,7 +1338,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1389,7 +1374,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1431,7 +1416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1439,23 +1424,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1489,11 +1474,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1531,7 +1516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1569,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1607,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1645,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1681,7 +1666,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1717,7 +1702,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1753,7 +1738,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1789,7 +1774,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1825,7 +1810,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1861,7 +1846,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1897,7 +1882,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -1933,7 +1918,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -1969,7 +1954,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -2005,7 +1990,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>5</v>
       </c>
@@ -2041,7 +2026,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -2077,7 +2062,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>7</v>
       </c>
@@ -2113,7 +2098,7 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>8</v>
       </c>
@@ -2149,7 +2134,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>9</v>
       </c>
@@ -2185,7 +2170,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -2227,7 +2212,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2235,23 +2220,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2285,11 +2270,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2327,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2365,7 +2350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2403,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2441,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2477,7 +2462,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2513,7 +2498,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2549,7 +2534,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2585,7 +2570,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2621,7 +2606,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2657,7 +2642,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2693,7 +2678,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2729,7 +2714,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2765,7 +2750,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2801,7 +2786,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2837,7 +2822,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2873,7 +2858,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2909,7 +2894,7 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2945,7 +2930,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2981,7 +2966,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3017,7 +3002,7 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3053,7 +3038,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3089,7 +3074,7 @@
       </c>
       <c r="L23" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3125,7 +3110,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3161,7 +3146,7 @@
       </c>
       <c r="L25" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3197,7 +3182,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3233,7 +3218,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3269,7 +3254,7 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3305,7 +3290,7 @@
       </c>
       <c r="L29" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3341,7 +3326,7 @@
       </c>
       <c r="L30" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3377,7 +3362,7 @@
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3413,7 +3398,7 @@
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3449,7 +3434,7 @@
       </c>
       <c r="L33" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3485,7 +3470,7 @@
       </c>
       <c r="L34" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3521,7 +3506,7 @@
       </c>
       <c r="L35" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3557,7 +3542,7 @@
       </c>
       <c r="L36" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3593,7 +3578,7 @@
       </c>
       <c r="L37" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3629,7 +3614,7 @@
       </c>
       <c r="L38" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3665,7 +3650,7 @@
       </c>
       <c r="L39" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3701,7 +3686,7 @@
       </c>
       <c r="L40" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3737,7 +3722,7 @@
       </c>
       <c r="L41" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3773,7 +3758,7 @@
       </c>
       <c r="L42" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3809,7 +3794,7 @@
       </c>
       <c r="L43" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3845,7 +3830,7 @@
       </c>
       <c r="L44" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3881,7 +3866,7 @@
       </c>
       <c r="L45" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3917,7 +3902,7 @@
       </c>
       <c r="L46" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3953,7 +3938,7 @@
       </c>
       <c r="L47" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3989,7 +3974,7 @@
       </c>
       <c r="L48" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -4025,7 +4010,7 @@
       </c>
       <c r="L49" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -4061,7 +4046,7 @@
       </c>
       <c r="L50" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -4097,7 +4082,7 @@
       </c>
       <c r="L51" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -4133,7 +4118,7 @@
       </c>
       <c r="L52" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -4169,7 +4154,7 @@
       </c>
       <c r="L53" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -4205,7 +4190,7 @@
       </c>
       <c r="L54" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -4241,7 +4226,7 @@
       </c>
       <c r="L55" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -4277,7 +4262,7 @@
       </c>
       <c r="L56" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4313,7 +4298,7 @@
       </c>
       <c r="L57" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4349,7 +4334,7 @@
       </c>
       <c r="L58" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4385,7 +4370,7 @@
       </c>
       <c r="L59" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4421,7 +4406,7 @@
       </c>
       <c r="L60" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4463,7 +4448,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4471,23 +4456,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4503,33 +4488,33 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1">
@@ -4541,21 +4526,15 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
       <c r="L2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1">
@@ -4567,21 +4546,15 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
       <c r="L3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1">
@@ -4593,21 +4566,15 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
       <c r="L4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1">
@@ -4619,21 +4586,15 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
       <c r="L5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1">
@@ -4645,19 +4606,13 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
       <c r="L6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1">
@@ -4669,19 +4624,13 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
       <c r="L7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1">
@@ -4693,19 +4642,13 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
       <c r="L8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1">
@@ -4717,19 +4660,13 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
       <c r="L9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1">
@@ -4741,19 +4678,13 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
       <c r="L10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1">
@@ -4765,19 +4696,13 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
       <c r="L11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1">
@@ -4789,19 +4714,13 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
       <c r="L12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1">
@@ -4813,19 +4732,13 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
       <c r="L13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1">
@@ -4837,19 +4750,13 @@
       <c r="E14" s="1">
         <v>0</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
       <c r="L14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1">
@@ -4861,19 +4768,13 @@
       <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
       <c r="L15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1">
@@ -4885,19 +4786,13 @@
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
       <c r="L16" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="1">
@@ -4909,19 +4804,13 @@
       <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
       <c r="L17" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="1">
@@ -4933,19 +4822,13 @@
       <c r="E18" s="1">
         <v>0</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
       <c r="L18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="1">
@@ -4957,19 +4840,13 @@
       <c r="E19" s="1">
         <v>0</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
       <c r="L19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="1">
@@ -4981,19 +4858,13 @@
       <c r="E20" s="1">
         <v>0</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
       <c r="L20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1">
@@ -5005,12 +4876,6 @@
       <c r="E21" s="1">
         <v>0</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
       <c r="L21" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel for trials
</commit_message>
<xml_diff>
--- a/Trials.xlsx
+++ b/Trials.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/155826a8f07387bf/GE_Drive/PhD/PhD Projects/codes/unimanual-codes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_7341B9EB30DD48EF078EC3732D2B8AD49365BD76" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2E36EF4-A0B7-4221-B0E8-8B24D6297F1D}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="720" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Template"/>
-    <sheet r:id="rId2" sheetId="2" name="Testing"/>
-    <sheet r:id="rId3" sheetId="3" name="Practice"/>
-    <sheet r:id="rId4" sheetId="4" name="Baseline"/>
-    <sheet r:id="rId5" sheetId="5" name="Exposure"/>
-    <sheet r:id="rId6" sheetId="6" name="Post"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Testing" sheetId="2" r:id="rId2"/>
+    <sheet name="Practice" sheetId="3" r:id="rId3"/>
+    <sheet name="Baseline" sheetId="4" r:id="rId4"/>
+    <sheet name="Exposure" sheetId="5" r:id="rId5"/>
+    <sheet name="Post" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -123,8 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,12 +154,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdeebf7"/>
+        <fgColor rgb="FFDEEBF7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFfff2cc"/>
+        <fgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -192,59 +197,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -255,10 +257,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -296,71 +298,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -388,7 +390,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -411,11 +413,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -424,13 +426,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -440,7 +442,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -449,7 +451,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -458,7 +460,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -466,10 +468,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -534,7 +536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -542,223 +544,210 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="15.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="14" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="14" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="14" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="16.109375" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+    </row>
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+    </row>
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+    </row>
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+    </row>
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -766,31 +755,33 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,7 +819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -857,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="J2" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K2" s="1">
         <v>0</v>
@@ -866,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -895,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>
@@ -904,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -933,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
@@ -942,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -971,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
@@ -980,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1009,7 +1000,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K6" s="1">
         <v>0</v>
@@ -1018,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1047,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="J7" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
@@ -1056,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1085,12 +1076,658 @@
         <v>0</v>
       </c>
       <c r="J8" s="1">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
       </c>
       <c r="L8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1100,7 +1737,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1108,23 +1745,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1158,11 +1795,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1200,7 +1837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1238,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1276,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1314,7 +1951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1350,7 +1987,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1386,7 +2023,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1422,7 +2059,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1458,7 +2095,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1494,7 +2131,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1536,7 +2173,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1544,23 +2181,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1594,11 +2231,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1636,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1674,7 +2311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1712,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1750,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1786,7 +2423,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1822,7 +2459,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1858,7 +2495,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1894,7 +2531,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1930,7 +2567,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1966,7 +2603,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -2002,7 +2639,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -2038,7 +2675,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -2074,7 +2711,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>4</v>
       </c>
@@ -2110,7 +2747,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>5</v>
       </c>
@@ -2146,7 +2783,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -2182,7 +2819,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>7</v>
       </c>
@@ -2218,7 +2855,7 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>8</v>
       </c>
@@ -2254,7 +2891,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>9</v>
       </c>
@@ -2290,7 +2927,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>10</v>
       </c>
@@ -2332,7 +2969,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2340,23 +2977,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2390,11 +3027,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2432,7 +3069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2470,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2508,7 +3145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2546,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2582,7 +3219,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2618,7 +3255,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2654,7 +3291,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2690,7 +3327,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2726,7 +3363,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2762,7 +3399,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2798,7 +3435,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2834,7 +3471,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2870,7 +3507,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2906,7 +3543,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2942,7 +3579,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2978,7 +3615,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3014,7 +3651,7 @@
       </c>
       <c r="L18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -3050,7 +3687,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -3086,7 +3723,7 @@
       </c>
       <c r="L20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -3122,7 +3759,7 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -3158,7 +3795,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -3194,7 +3831,7 @@
       </c>
       <c r="L23" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -3230,7 +3867,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -3266,7 +3903,7 @@
       </c>
       <c r="L25" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -3302,7 +3939,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -3338,7 +3975,7 @@
       </c>
       <c r="L27" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -3374,7 +4011,7 @@
       </c>
       <c r="L28" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -3410,7 +4047,7 @@
       </c>
       <c r="L29" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -3446,7 +4083,7 @@
       </c>
       <c r="L30" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -3482,7 +4119,7 @@
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -3518,7 +4155,7 @@
       </c>
       <c r="L32" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -3554,7 +4191,7 @@
       </c>
       <c r="L33" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3590,7 +4227,7 @@
       </c>
       <c r="L34" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3626,7 +4263,7 @@
       </c>
       <c r="L35" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3662,7 +4299,7 @@
       </c>
       <c r="L36" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3698,7 +4335,7 @@
       </c>
       <c r="L37" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3734,7 +4371,7 @@
       </c>
       <c r="L38" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3770,7 +4407,7 @@
       </c>
       <c r="L39" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3806,7 +4443,7 @@
       </c>
       <c r="L40" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3842,7 +4479,7 @@
       </c>
       <c r="L41" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3878,7 +4515,7 @@
       </c>
       <c r="L42" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3914,7 +4551,7 @@
       </c>
       <c r="L43" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3950,7 +4587,7 @@
       </c>
       <c r="L44" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3986,7 +4623,7 @@
       </c>
       <c r="L45" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -4022,7 +4659,7 @@
       </c>
       <c r="L46" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -4058,7 +4695,7 @@
       </c>
       <c r="L47" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -4094,7 +4731,7 @@
       </c>
       <c r="L48" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -4130,7 +4767,7 @@
       </c>
       <c r="L49" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -4166,7 +4803,7 @@
       </c>
       <c r="L50" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -4202,7 +4839,7 @@
       </c>
       <c r="L51" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -4238,7 +4875,7 @@
       </c>
       <c r="L52" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -4274,7 +4911,7 @@
       </c>
       <c r="L53" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -4310,7 +4947,7 @@
       </c>
       <c r="L54" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -4346,7 +4983,7 @@
       </c>
       <c r="L55" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -4382,7 +5019,7 @@
       </c>
       <c r="L56" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4418,7 +5055,7 @@
       </c>
       <c r="L57" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4454,7 +5091,7 @@
       </c>
       <c r="L58" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4490,7 +5127,7 @@
       </c>
       <c r="L59" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4526,7 +5163,7 @@
       </c>
       <c r="L60" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4568,7 +5205,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -4576,23 +5213,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="10.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="18.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="17.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="6.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4608,33 +5245,33 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="1">
@@ -4646,21 +5283,15 @@
       <c r="E2" s="1">
         <v>0</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
       <c r="L2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="1">
@@ -4672,21 +5303,15 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
       <c r="L3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1">
@@ -4698,21 +5323,15 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
       <c r="L4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1">
@@ -4724,21 +5343,15 @@
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
       <c r="L5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1">
@@ -4750,19 +5363,13 @@
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
       <c r="L6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="1">
@@ -4774,19 +5381,13 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
       <c r="L7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1">
@@ -4798,19 +5399,13 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
       <c r="L8" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1">
@@ -4822,19 +5417,13 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
       <c r="L9" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1">
@@ -4846,19 +5435,13 @@
       <c r="E10" s="1">
         <v>0</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
       <c r="L10" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="1">
@@ -4870,19 +5453,13 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
       <c r="L11" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1">
@@ -4894,19 +5471,13 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
       <c r="L12" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1">
@@ -4918,19 +5489,13 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
       <c r="L13" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1">
@@ -4942,19 +5507,13 @@
       <c r="E14" s="1">
         <v>0</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
       <c r="L14" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="1">
@@ -4966,19 +5525,13 @@
       <c r="E15" s="1">
         <v>0</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
       <c r="L15" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1">
@@ -4990,19 +5543,13 @@
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
       <c r="L16" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="1">
@@ -5014,19 +5561,13 @@
       <c r="E17" s="1">
         <v>0</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
       <c r="L17" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="1">
@@ -5038,19 +5579,13 @@
       <c r="E18" s="1">
         <v>0</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
       <c r="L18" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="1">
@@ -5062,19 +5597,13 @@
       <c r="E19" s="1">
         <v>0</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
       <c r="L19" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="1">
@@ -5086,19 +5615,13 @@
       <c r="E20" s="1">
         <v>0</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
       <c r="L20" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1">
@@ -5110,12 +5633,6 @@
       <c r="E21" s="1">
         <v>0</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
       <c r="L21" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change to saving protocols to all csv, and update file paths to fstrings
</commit_message>
<xml_diff>
--- a/Trials.xlsx
+++ b/Trials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/155826a8f07387bf/GE_Drive/PhD/PhD Projects/general-code/unimanual-codes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/155826a8f07387bf/GE_Drive/PhD/PhD Projects/Project 1 Vibration Adaptation/Study 2 Vibration Adaptation with Vision/vibration-adaptation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="11_0D7C4CB69DB6445E418EC6DC411670CC1F04352D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{420EE078-1A58-4D4F-9B85-6D527061254D}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_0D7C4CB69DB6445E418EC6DC411670CC1F04352D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F21294E7-F223-46A5-B1D7-5E78C326FCD6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="trial-randomizer" sheetId="7" r:id="rId1"/>
@@ -21,8 +21,19 @@
     <sheet name="Exposure" sheetId="5" r:id="rId6"/>
     <sheet name="Post" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -322,10 +333,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -501,14 +508,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58274492-96F2-4057-A8B5-0AFD831A14C2}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <f ca="1">RAND()</f>
+        <v>0.56470351761664395</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f ca="1">RAND()</f>
+        <v>0.24613987209079013</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f ca="1">RAND()</f>
+        <v>0.44146005160748958</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f ca="1">RAND()</f>
+        <v>0.87159941682023323</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C5">
+    <sortCondition ref="C2:C5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1426,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="10">
         <v>0</v>
@@ -1530,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="10">
         <v>0</v>
@@ -1606,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="10">
         <v>0</v>
@@ -1644,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
@@ -1682,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="10">
         <v>0</v>
@@ -1758,7 +1805,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="10">
         <v>0</v>
@@ -1796,7 +1843,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="10">
         <v>0</v>
@@ -1834,7 +1881,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" s="10">
         <v>0</v>
@@ -1872,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="10">
         <v>0</v>
@@ -2024,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" s="10">
         <v>0</v>
@@ -2062,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" s="10">
         <v>0</v>
@@ -2214,7 +2261,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D21" s="10">
         <v>0</v>
@@ -2245,42 +2292,17 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>20</v>
-      </c>
-      <c r="B22" s="10">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9">
-        <v>3</v>
-      </c>
-      <c r="D22" s="10">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10">
-        <v>1</v>
-      </c>
-      <c r="F22" s="10">
-        <v>0</v>
-      </c>
-      <c r="G22" s="10">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10">
-        <v>0</v>
-      </c>
-      <c r="I22" s="10">
-        <v>0</v>
-      </c>
-      <c r="J22" s="10">
-        <v>0</v>
-      </c>
-      <c r="K22" s="10">
-        <v>0</v>
-      </c>
-      <c r="L22" s="10">
-        <v>0</v>
-      </c>
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2290,10 +2312,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,7 +2380,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="10">
         <v>0</v>
@@ -2381,8 +2403,8 @@
       <c r="J2" s="10">
         <v>0</v>
       </c>
-      <c r="K2" s="10">
-        <v>0</v>
+      <c r="K2">
+        <v>1</v>
       </c>
       <c r="L2" s="10">
         <v>0</v>
@@ -2396,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="10">
         <v>0</v>
@@ -2419,7 +2441,7 @@
       <c r="J3" s="10">
         <v>0</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3">
         <v>0</v>
       </c>
       <c r="L3" s="10">
@@ -2457,8 +2479,8 @@
       <c r="J4" s="10">
         <v>0</v>
       </c>
-      <c r="K4" s="10">
-        <v>0</v>
+      <c r="K4">
+        <v>3</v>
       </c>
       <c r="L4" s="10">
         <v>0</v>
@@ -2495,8 +2517,8 @@
       <c r="J5" s="10">
         <v>0</v>
       </c>
-      <c r="K5" s="10">
-        <v>0</v>
+      <c r="K5">
+        <v>2</v>
       </c>
       <c r="L5" s="10">
         <v>0</v>
@@ -2510,7 +2532,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="10">
         <v>0</v>
@@ -2533,8 +2555,8 @@
       <c r="J6" s="10">
         <v>0</v>
       </c>
-      <c r="K6" s="10">
-        <v>0</v>
+      <c r="K6">
+        <v>3</v>
       </c>
       <c r="L6" s="10">
         <v>0</v>
@@ -2548,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7" s="10">
         <v>0</v>
@@ -2571,7 +2593,7 @@
       <c r="J7" s="10">
         <v>0</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7">
         <v>0</v>
       </c>
       <c r="L7" s="10">
@@ -2586,31 +2608,31 @@
         <v>0</v>
       </c>
       <c r="C8" s="10">
+        <v>3</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>2</v>
-      </c>
-      <c r="D8" s="10">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10">
-        <v>0</v>
-      </c>
-      <c r="F8" s="10">
-        <v>0</v>
-      </c>
-      <c r="G8" s="10">
-        <v>0</v>
-      </c>
-      <c r="H8" s="10">
-        <v>0</v>
-      </c>
-      <c r="I8" s="10">
-        <v>0</v>
-      </c>
-      <c r="J8" s="10">
-        <v>0</v>
-      </c>
-      <c r="K8" s="10">
-        <v>0</v>
       </c>
       <c r="L8" s="10">
         <v>0</v>
@@ -2647,8 +2669,8 @@
       <c r="J9" s="10">
         <v>0</v>
       </c>
-      <c r="K9" s="10">
-        <v>0</v>
+      <c r="K9">
+        <v>1</v>
       </c>
       <c r="L9" s="10">
         <v>0</v>
@@ -2662,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D10" s="10">
         <v>0</v>
@@ -2685,8 +2707,8 @@
       <c r="J10" s="10">
         <v>0</v>
       </c>
-      <c r="K10" s="10">
-        <v>0</v>
+      <c r="K10">
+        <v>1</v>
       </c>
       <c r="L10" s="10">
         <v>0</v>
@@ -2700,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D11" s="10">
         <v>0</v>
@@ -2723,8 +2745,8 @@
       <c r="J11" s="10">
         <v>0</v>
       </c>
-      <c r="K11" s="10">
-        <v>0</v>
+      <c r="K11">
+        <v>2</v>
       </c>
       <c r="L11" s="10">
         <v>0</v>
@@ -2761,7 +2783,7 @@
       <c r="J12" s="10">
         <v>0</v>
       </c>
-      <c r="K12" s="10">
+      <c r="K12">
         <v>0</v>
       </c>
       <c r="L12" s="10">
@@ -2776,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="10">
         <v>0</v>
@@ -2799,8 +2821,8 @@
       <c r="J13" s="10">
         <v>0</v>
       </c>
-      <c r="K13" s="10">
-        <v>0</v>
+      <c r="K13">
+        <v>3</v>
       </c>
       <c r="L13" s="10">
         <v>0</v>
@@ -2837,8 +2859,8 @@
       <c r="J14" s="10">
         <v>0</v>
       </c>
-      <c r="K14" s="10">
-        <v>0</v>
+      <c r="K14">
+        <v>1</v>
       </c>
       <c r="L14" s="10">
         <v>0</v>
@@ -2852,7 +2874,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" s="10">
         <v>0</v>
@@ -2875,8 +2897,8 @@
       <c r="J15" s="10">
         <v>0</v>
       </c>
-      <c r="K15" s="10">
-        <v>0</v>
+      <c r="K15">
+        <v>3</v>
       </c>
       <c r="L15" s="10">
         <v>0</v>
@@ -2890,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16" s="10">
         <v>0</v>
@@ -2913,7 +2935,7 @@
       <c r="J16" s="10">
         <v>0</v>
       </c>
-      <c r="K16" s="10">
+      <c r="K16">
         <v>0</v>
       </c>
       <c r="L16" s="10">
@@ -2928,7 +2950,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" s="10">
         <v>0</v>
@@ -2951,8 +2973,8 @@
       <c r="J17" s="10">
         <v>0</v>
       </c>
-      <c r="K17" s="10">
-        <v>0</v>
+      <c r="K17">
+        <v>2</v>
       </c>
       <c r="L17" s="10">
         <v>0</v>
@@ -2966,7 +2988,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D18" s="10">
         <v>0</v>
@@ -2989,8 +3011,8 @@
       <c r="J18" s="10">
         <v>0</v>
       </c>
-      <c r="K18" s="10">
-        <v>0</v>
+      <c r="K18">
+        <v>1</v>
       </c>
       <c r="L18" s="10">
         <v>0</v>
@@ -3027,8 +3049,8 @@
       <c r="J19" s="10">
         <v>0</v>
       </c>
-      <c r="K19" s="10">
-        <v>0</v>
+      <c r="K19">
+        <v>2</v>
       </c>
       <c r="L19" s="10">
         <v>0</v>
@@ -3042,7 +3064,7 @@
         <v>0</v>
       </c>
       <c r="C20" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D20" s="10">
         <v>0</v>
@@ -3065,7 +3087,7 @@
       <c r="J20" s="10">
         <v>0</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20">
         <v>0</v>
       </c>
       <c r="L20" s="10">
@@ -3080,7 +3102,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D21" s="10">
         <v>0</v>
@@ -3103,8 +3125,8 @@
       <c r="J21" s="10">
         <v>0</v>
       </c>
-      <c r="K21" s="10">
-        <v>0</v>
+      <c r="K21">
+        <v>3</v>
       </c>
       <c r="L21" s="10">
         <v>0</v>
@@ -3112,7 +3134,7 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="10">
         <v>0</v>
@@ -3141,10 +3163,732 @@
       <c r="J22" s="10">
         <v>0</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22">
         <v>0</v>
       </c>
       <c r="L22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="10">
+        <v>0</v>
+      </c>
+      <c r="C23" s="9">
+        <v>3</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0</v>
+      </c>
+      <c r="G23" s="10">
+        <v>0</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0</v>
+      </c>
+      <c r="J23" s="10">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="10">
+        <v>0</v>
+      </c>
+      <c r="C24" s="9">
+        <v>3</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0</v>
+      </c>
+      <c r="F24" s="10">
+        <v>0</v>
+      </c>
+      <c r="G24" s="10">
+        <v>0</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0</v>
+      </c>
+      <c r="I24" s="10">
+        <v>0</v>
+      </c>
+      <c r="J24" s="10">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>24</v>
+      </c>
+      <c r="B25" s="10">
+        <v>0</v>
+      </c>
+      <c r="C25" s="9">
+        <v>3</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0</v>
+      </c>
+      <c r="F25" s="10">
+        <v>0</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0</v>
+      </c>
+      <c r="I25" s="10">
+        <v>0</v>
+      </c>
+      <c r="J25" s="10">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="10">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9">
+        <v>3</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0</v>
+      </c>
+      <c r="F26" s="10">
+        <v>0</v>
+      </c>
+      <c r="G26" s="10">
+        <v>0</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0</v>
+      </c>
+      <c r="J26" s="10">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>26</v>
+      </c>
+      <c r="B27" s="10">
+        <v>0</v>
+      </c>
+      <c r="C27" s="9">
+        <v>3</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0</v>
+      </c>
+      <c r="G27" s="10">
+        <v>0</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+      <c r="I27" s="10">
+        <v>0</v>
+      </c>
+      <c r="J27" s="10">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="L27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="B28" s="10">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9">
+        <v>3</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+      <c r="I28" s="10">
+        <v>0</v>
+      </c>
+      <c r="J28" s="10">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>28</v>
+      </c>
+      <c r="B29" s="10">
+        <v>0</v>
+      </c>
+      <c r="C29" s="9">
+        <v>3</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0</v>
+      </c>
+      <c r="J29" s="10">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>2</v>
+      </c>
+      <c r="L29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>29</v>
+      </c>
+      <c r="B30" s="10">
+        <v>0</v>
+      </c>
+      <c r="C30" s="9">
+        <v>3</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0</v>
+      </c>
+      <c r="E30" s="10">
+        <v>0</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0</v>
+      </c>
+      <c r="I30" s="10">
+        <v>0</v>
+      </c>
+      <c r="J30" s="10">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="L30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>30</v>
+      </c>
+      <c r="B31" s="10">
+        <v>0</v>
+      </c>
+      <c r="C31" s="9">
+        <v>3</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0</v>
+      </c>
+      <c r="H31" s="10">
+        <v>0</v>
+      </c>
+      <c r="I31" s="10">
+        <v>0</v>
+      </c>
+      <c r="J31" s="10">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>2</v>
+      </c>
+      <c r="L31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>31</v>
+      </c>
+      <c r="B32" s="10">
+        <v>0</v>
+      </c>
+      <c r="C32" s="9">
+        <v>3</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0</v>
+      </c>
+      <c r="G32" s="10">
+        <v>0</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0</v>
+      </c>
+      <c r="I32" s="10">
+        <v>0</v>
+      </c>
+      <c r="J32" s="10">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>32</v>
+      </c>
+      <c r="B33" s="10">
+        <v>0</v>
+      </c>
+      <c r="C33" s="9">
+        <v>3</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0</v>
+      </c>
+      <c r="E33" s="10">
+        <v>0</v>
+      </c>
+      <c r="F33" s="10">
+        <v>0</v>
+      </c>
+      <c r="G33" s="10">
+        <v>0</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0</v>
+      </c>
+      <c r="I33" s="10">
+        <v>0</v>
+      </c>
+      <c r="J33" s="10">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>3</v>
+      </c>
+      <c r="L33" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>33</v>
+      </c>
+      <c r="B34" s="10">
+        <v>0</v>
+      </c>
+      <c r="C34" s="9">
+        <v>3</v>
+      </c>
+      <c r="D34" s="10">
+        <v>0</v>
+      </c>
+      <c r="E34" s="10">
+        <v>0</v>
+      </c>
+      <c r="F34" s="10">
+        <v>0</v>
+      </c>
+      <c r="G34" s="10">
+        <v>0</v>
+      </c>
+      <c r="H34" s="10">
+        <v>0</v>
+      </c>
+      <c r="I34" s="10">
+        <v>0</v>
+      </c>
+      <c r="J34" s="10">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>2</v>
+      </c>
+      <c r="L34" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>34</v>
+      </c>
+      <c r="B35" s="10">
+        <v>0</v>
+      </c>
+      <c r="C35" s="9">
+        <v>3</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0</v>
+      </c>
+      <c r="E35" s="10">
+        <v>0</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10">
+        <v>0</v>
+      </c>
+      <c r="H35" s="10">
+        <v>0</v>
+      </c>
+      <c r="I35" s="10">
+        <v>0</v>
+      </c>
+      <c r="J35" s="10">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>35</v>
+      </c>
+      <c r="B36" s="10">
+        <v>0</v>
+      </c>
+      <c r="C36" s="9">
+        <v>3</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0</v>
+      </c>
+      <c r="E36" s="10">
+        <v>0</v>
+      </c>
+      <c r="F36" s="10">
+        <v>0</v>
+      </c>
+      <c r="G36" s="10">
+        <v>0</v>
+      </c>
+      <c r="H36" s="10">
+        <v>0</v>
+      </c>
+      <c r="I36" s="10">
+        <v>0</v>
+      </c>
+      <c r="J36" s="10">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>3</v>
+      </c>
+      <c r="L36" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10">
+        <v>0</v>
+      </c>
+      <c r="C37" s="9">
+        <v>3</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10">
+        <v>0</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0</v>
+      </c>
+      <c r="H37" s="10">
+        <v>0</v>
+      </c>
+      <c r="I37" s="10">
+        <v>0</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>37</v>
+      </c>
+      <c r="B38" s="10">
+        <v>0</v>
+      </c>
+      <c r="C38" s="9">
+        <v>3</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0</v>
+      </c>
+      <c r="E38" s="10">
+        <v>0</v>
+      </c>
+      <c r="F38" s="10">
+        <v>0</v>
+      </c>
+      <c r="G38" s="10">
+        <v>0</v>
+      </c>
+      <c r="H38" s="10">
+        <v>0</v>
+      </c>
+      <c r="I38" s="10">
+        <v>0</v>
+      </c>
+      <c r="J38" s="10">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>3</v>
+      </c>
+      <c r="L38" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>38</v>
+      </c>
+      <c r="B39" s="10">
+        <v>0</v>
+      </c>
+      <c r="C39" s="9">
+        <v>3</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0</v>
+      </c>
+      <c r="E39" s="10">
+        <v>0</v>
+      </c>
+      <c r="F39" s="10">
+        <v>0</v>
+      </c>
+      <c r="G39" s="10">
+        <v>0</v>
+      </c>
+      <c r="H39" s="10">
+        <v>0</v>
+      </c>
+      <c r="I39" s="10">
+        <v>0</v>
+      </c>
+      <c r="J39" s="10">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+      <c r="L39" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10">
+        <v>0</v>
+      </c>
+      <c r="C40" s="9">
+        <v>3</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0</v>
+      </c>
+      <c r="E40" s="10">
+        <v>0</v>
+      </c>
+      <c r="F40" s="10">
+        <v>0</v>
+      </c>
+      <c r="G40" s="10">
+        <v>0</v>
+      </c>
+      <c r="H40" s="10">
+        <v>0</v>
+      </c>
+      <c r="I40" s="10">
+        <v>0</v>
+      </c>
+      <c r="J40" s="10">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>40</v>
+      </c>
+      <c r="B41" s="10">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9">
+        <v>3</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10">
+        <v>0</v>
+      </c>
+      <c r="G41" s="10">
+        <v>0</v>
+      </c>
+      <c r="H41" s="10">
+        <v>0</v>
+      </c>
+      <c r="I41" s="10">
+        <v>0</v>
+      </c>
+      <c r="J41" s="10">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>2</v>
+      </c>
+      <c r="L41" s="10">
         <v>0</v>
       </c>
     </row>

</xml_diff>